<commit_message>
Adjusted HUMAN NEXTCLADE Module and added REPORT module to HUMAN workflow
</commit_message>
<xml_diff>
--- a/assets/Inhibtion_Mutations_of_Intrest_2324.xlsx
+++ b/assets/Inhibtion_Mutations_of_Intrest_2324.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Virologi\NGS\1-NGS-Analyser\1-Rutine\2-Resultater\Influensa\Sesongfiler\2324\Mutation_lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A22E0A-40BD-44CC-9C93-EDCC57BAD4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDEB30A-78AB-4321-8E2A-42DD3168492D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26610" yWindow="765" windowWidth="23145" windowHeight="19545" xr2:uid="{0D809499-6AB2-485B-B1B9-717479A0DA7D}"/>
+    <workbookView xWindow="960" yWindow="270" windowWidth="30270" windowHeight="18165" xr2:uid="{0D809499-6AB2-485B-B1B9-717479A0DA7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -1730,9 +1730,6 @@
     <t>L38F</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>Amantadine</t>
   </si>
   <si>
@@ -1800,6 +1797,9 @@
   </si>
   <si>
     <t>E120D</t>
+  </si>
+  <si>
+    <t>M2</t>
   </si>
 </sst>
 </file>
@@ -2164,8 +2164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5CB93AC-71EE-42C9-B83A-09F5105723E2}">
   <dimension ref="A1:I262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
-      <selection activeCell="E259" sqref="E259"/>
+    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="F211" sqref="F211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2206,7 +2206,7 @@
         <v>220</v>
       </c>
       <c r="I1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -6653,7 +6653,7 @@
         <v>558</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>564</v>
+        <v>587</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>14</v>
@@ -6664,7 +6664,7 @@
         <v>559</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>564</v>
+        <v>587</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>14</v>
@@ -6675,7 +6675,7 @@
         <v>560</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>564</v>
+        <v>587</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>14</v>
@@ -6686,7 +6686,7 @@
         <v>561</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>564</v>
+        <v>587</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>14</v>
@@ -6697,7 +6697,7 @@
         <v>562</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>564</v>
+        <v>587</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>14</v>
@@ -6708,7 +6708,7 @@
         <v>563</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>564</v>
+        <v>587</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>14</v>
@@ -6719,7 +6719,7 @@
         <v>558</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>564</v>
+        <v>587</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>330</v>
@@ -6730,7 +6730,7 @@
         <v>559</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>564</v>
+        <v>587</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>330</v>
@@ -6741,7 +6741,7 @@
         <v>560</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>564</v>
+        <v>587</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>330</v>
@@ -6752,7 +6752,7 @@
         <v>561</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>564</v>
+        <v>587</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>330</v>
@@ -6763,7 +6763,7 @@
         <v>562</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>564</v>
+        <v>587</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>330</v>
@@ -6774,7 +6774,7 @@
         <v>563</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>564</v>
+        <v>587</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>330</v>
@@ -6785,7 +6785,7 @@
         <v>558</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>564</v>
+        <v>587</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>3</v>
@@ -6796,7 +6796,7 @@
         <v>559</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>564</v>
+        <v>587</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>3</v>
@@ -6807,7 +6807,7 @@
         <v>560</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>564</v>
+        <v>587</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>3</v>
@@ -6818,7 +6818,7 @@
         <v>561</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>564</v>
+        <v>587</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>3</v>
@@ -6829,7 +6829,7 @@
         <v>562</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>564</v>
+        <v>587</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>3</v>
@@ -6840,7 +6840,7 @@
         <v>563</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>564</v>
+        <v>587</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>3</v>
@@ -6848,10 +6848,10 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>14</v>
@@ -6859,10 +6859,10 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>14</v>
@@ -6870,10 +6870,10 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>14</v>
@@ -6881,10 +6881,10 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>14</v>
@@ -6892,10 +6892,10 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>14</v>
@@ -6903,10 +6903,10 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>14</v>
@@ -6914,10 +6914,10 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>14</v>
@@ -6925,10 +6925,10 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>14</v>
@@ -6936,10 +6936,10 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>14</v>
@@ -6950,7 +6950,7 @@
         <v>7</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>14</v>
@@ -6958,10 +6958,10 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>14</v>
@@ -6969,10 +6969,10 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>14</v>
@@ -6980,10 +6980,10 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>14</v>
@@ -6991,10 +6991,10 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>14</v>
@@ -7002,10 +7002,10 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>14</v>
@@ -7013,10 +7013,10 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>14</v>
@@ -7024,10 +7024,10 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>14</v>
@@ -7035,10 +7035,10 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>14</v>
@@ -7046,10 +7046,10 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>14</v>
@@ -7057,10 +7057,10 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>14</v>
@@ -7068,10 +7068,10 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>14</v>
@@ -7079,10 +7079,10 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>14</v>
@@ -7090,10 +7090,10 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>14</v>
@@ -7101,10 +7101,10 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>14</v>
@@ -7112,10 +7112,10 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
+        <v>580</v>
+      </c>
+      <c r="B236" s="1" t="s">
         <v>581</v>
-      </c>
-      <c r="B236" s="1" t="s">
-        <v>582</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>14</v>
@@ -7123,10 +7123,10 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>330</v>
@@ -7134,10 +7134,10 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>330</v>
@@ -7145,10 +7145,10 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>330</v>
@@ -7156,10 +7156,10 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C240" s="1" t="s">
         <v>330</v>
@@ -7167,10 +7167,10 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>330</v>
@@ -7178,10 +7178,10 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>330</v>
@@ -7189,10 +7189,10 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>330</v>
@@ -7200,10 +7200,10 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>330</v>
@@ -7211,10 +7211,10 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>330</v>
@@ -7222,10 +7222,10 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>330</v>
@@ -7233,10 +7233,10 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>330</v>
@@ -7244,10 +7244,10 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>330</v>
@@ -7255,10 +7255,10 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>330</v>
@@ -7266,10 +7266,10 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>330</v>
@@ -7280,7 +7280,7 @@
         <v>7</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>330</v>
@@ -7288,10 +7288,10 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>330</v>
@@ -7299,10 +7299,10 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
+        <v>580</v>
+      </c>
+      <c r="B253" s="1" t="s">
         <v>581</v>
-      </c>
-      <c r="B253" s="1" t="s">
-        <v>582</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>330</v>
@@ -7310,10 +7310,10 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>557</v>
@@ -7321,10 +7321,10 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>557</v>
@@ -7332,10 +7332,10 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>557</v>
@@ -7343,10 +7343,10 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>557</v>
@@ -7354,10 +7354,10 @@
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>557</v>
@@ -7365,10 +7365,10 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>557</v>
@@ -7376,10 +7376,10 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>557</v>
@@ -7387,10 +7387,10 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>557</v>
@@ -7398,10 +7398,10 @@
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>557</v>

</xml_diff>

<commit_message>
Added Influenza Victoria to HUMAN workflow and ouput filtered fasta
</commit_message>
<xml_diff>
--- a/assets/Inhibtion_Mutations_of_Intrest_2324.xlsx
+++ b/assets/Inhibtion_Mutations_of_Intrest_2324.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Virologi\NGS\1-NGS-Analyser\1-Rutine\2-Resultater\Influensa\Sesongfiler\2324\Mutation_lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDEB30A-78AB-4321-8E2A-42DD3168492D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448ABC34-0B88-447C-A77A-2409EBABB502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="270" windowWidth="30270" windowHeight="18165" xr2:uid="{0D809499-6AB2-485B-B1B9-717479A0DA7D}"/>
+    <workbookView xWindow="31275" yWindow="1095" windowWidth="19965" windowHeight="20535" xr2:uid="{0D809499-6AB2-485B-B1B9-717479A0DA7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -1709,9 +1709,6 @@
     <t>G247D;I361V</t>
   </si>
   <si>
-    <t>VIC</t>
-  </si>
-  <si>
     <t>L26F</t>
   </si>
   <si>
@@ -1800,6 +1797,9 @@
   </si>
   <si>
     <t>M2</t>
+  </si>
+  <si>
+    <t>VICVIC</t>
   </si>
 </sst>
 </file>
@@ -1818,7 +1818,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="204"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2164,8 +2164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5CB93AC-71EE-42C9-B83A-09F5105723E2}">
   <dimension ref="A1:I262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="F211" sqref="F211"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C254" sqref="C254:C262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2206,7 +2206,7 @@
         <v>220</v>
       </c>
       <c r="I1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -5345,7 +5345,7 @@
         <v>550</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>441</v>
@@ -5368,7 +5368,7 @@
         <v>550</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>445</v>
@@ -5391,7 +5391,7 @@
         <v>550</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>449</v>
@@ -5414,7 +5414,7 @@
         <v>550</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>453</v>
@@ -5437,7 +5437,7 @@
         <v>550</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>457</v>
@@ -5460,7 +5460,7 @@
         <v>550</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>461</v>
@@ -5483,7 +5483,7 @@
         <v>550</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>464</v>
@@ -5506,7 +5506,7 @@
         <v>550</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>215</v>
@@ -5529,7 +5529,7 @@
         <v>550</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E145" t="s">
         <v>329</v>
@@ -5552,7 +5552,7 @@
         <v>550</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E146" t="s">
         <v>105</v>
@@ -5575,7 +5575,7 @@
         <v>550</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E147" t="s">
         <v>111</v>
@@ -5598,7 +5598,7 @@
         <v>550</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E148" t="s">
         <v>77</v>
@@ -5621,7 +5621,7 @@
         <v>550</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E149" t="s">
         <v>475</v>
@@ -5644,7 +5644,7 @@
         <v>550</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E150" t="s">
         <v>479</v>
@@ -5667,7 +5667,7 @@
         <v>550</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E151" t="s">
         <v>108</v>
@@ -5690,7 +5690,7 @@
         <v>550</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E152" t="s">
         <v>77</v>
@@ -5713,7 +5713,7 @@
         <v>550</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E153" t="s">
         <v>441</v>
@@ -5736,7 +5736,7 @@
         <v>550</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E154" t="s">
         <v>108</v>
@@ -5759,7 +5759,7 @@
         <v>550</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E155" t="s">
         <v>486</v>
@@ -5782,7 +5782,7 @@
         <v>550</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E156" t="s">
         <v>490</v>
@@ -5805,7 +5805,7 @@
         <v>550</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E157" t="s">
         <v>493</v>
@@ -5828,7 +5828,7 @@
         <v>550</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E158" t="s">
         <v>77</v>
@@ -5851,7 +5851,7 @@
         <v>550</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E159" t="s">
         <v>325</v>
@@ -5874,7 +5874,7 @@
         <v>550</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E160" t="s">
         <v>472</v>
@@ -5897,7 +5897,7 @@
         <v>550</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E161" t="s">
         <v>108</v>
@@ -5920,7 +5920,7 @@
         <v>550</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E162" t="s">
         <v>497</v>
@@ -5943,7 +5943,7 @@
         <v>550</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E163" t="s">
         <v>105</v>
@@ -5966,7 +5966,7 @@
         <v>550</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E164" t="s">
         <v>449</v>
@@ -5989,7 +5989,7 @@
         <v>550</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E165" t="s">
         <v>502</v>
@@ -6012,7 +6012,7 @@
         <v>550</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E166" t="s">
         <v>504</v>
@@ -6035,7 +6035,7 @@
         <v>550</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E167" t="s">
         <v>508</v>
@@ -6058,7 +6058,7 @@
         <v>550</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E168" t="s">
         <v>511</v>
@@ -6081,7 +6081,7 @@
         <v>550</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E169" t="s">
         <v>514</v>
@@ -6104,7 +6104,7 @@
         <v>550</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E170" t="s">
         <v>108</v>
@@ -6127,7 +6127,7 @@
         <v>550</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E171" t="s">
         <v>519</v>
@@ -6150,7 +6150,7 @@
         <v>550</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E172" t="s">
         <v>108</v>
@@ -6173,7 +6173,7 @@
         <v>550</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E173" t="s">
         <v>111</v>
@@ -6196,7 +6196,7 @@
         <v>550</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E174" t="s">
         <v>524</v>
@@ -6219,7 +6219,7 @@
         <v>550</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E175" t="s">
         <v>461</v>
@@ -6242,7 +6242,7 @@
         <v>550</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E176" t="s">
         <v>527</v>
@@ -6265,7 +6265,7 @@
         <v>550</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E177" t="s">
         <v>108</v>
@@ -6288,7 +6288,7 @@
         <v>550</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E178" t="s">
         <v>108</v>
@@ -6311,7 +6311,7 @@
         <v>550</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E179" t="s">
         <v>531</v>
@@ -6334,7 +6334,7 @@
         <v>550</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E180" t="s">
         <v>325</v>
@@ -6357,7 +6357,7 @@
         <v>550</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E181" t="s">
         <v>105</v>
@@ -6380,7 +6380,7 @@
         <v>550</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E182" t="s">
         <v>111</v>
@@ -6403,7 +6403,7 @@
         <v>550</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E183" t="s">
         <v>77</v>
@@ -6426,7 +6426,7 @@
         <v>550</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E184" t="s">
         <v>77</v>
@@ -6449,7 +6449,7 @@
         <v>550</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E185" t="s">
         <v>536</v>
@@ -6472,7 +6472,7 @@
         <v>550</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E186" t="s">
         <v>77</v>
@@ -6495,7 +6495,7 @@
         <v>550</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E187" t="s">
         <v>77</v>
@@ -6518,7 +6518,7 @@
         <v>550</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E188" t="s">
         <v>111</v>
@@ -6541,7 +6541,7 @@
         <v>550</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E189" t="s">
         <v>107</v>
@@ -6564,7 +6564,7 @@
         <v>550</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E190" t="s">
         <v>325</v>
@@ -6587,7 +6587,7 @@
         <v>550</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E191" t="s">
         <v>542</v>
@@ -6610,7 +6610,7 @@
         <v>550</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E192" t="s">
         <v>105</v>
@@ -6633,7 +6633,7 @@
         <v>550</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E193" t="s">
         <v>546</v>
@@ -6650,10 +6650,10 @@
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>14</v>
@@ -6661,10 +6661,10 @@
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>14</v>
@@ -6672,10 +6672,10 @@
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>14</v>
@@ -6683,10 +6683,10 @@
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>14</v>
@@ -6694,10 +6694,10 @@
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>14</v>
@@ -6705,10 +6705,10 @@
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>14</v>
@@ -6716,10 +6716,10 @@
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>330</v>
@@ -6727,10 +6727,10 @@
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>330</v>
@@ -6738,10 +6738,10 @@
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>330</v>
@@ -6749,10 +6749,10 @@
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>330</v>
@@ -6760,10 +6760,10 @@
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>330</v>
@@ -6771,10 +6771,10 @@
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>330</v>
@@ -6782,10 +6782,10 @@
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>3</v>
@@ -6793,10 +6793,10 @@
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>3</v>
@@ -6804,10 +6804,10 @@
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>3</v>
@@ -6815,10 +6815,10 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>3</v>
@@ -6826,10 +6826,10 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>3</v>
@@ -6837,10 +6837,10 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>3</v>
@@ -6848,10 +6848,10 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>14</v>
@@ -6859,10 +6859,10 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>14</v>
@@ -6870,10 +6870,10 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>14</v>
@@ -6881,10 +6881,10 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>14</v>
@@ -6892,10 +6892,10 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>14</v>
@@ -6903,10 +6903,10 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>14</v>
@@ -6914,10 +6914,10 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>14</v>
@@ -6925,10 +6925,10 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>14</v>
@@ -6936,10 +6936,10 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>14</v>
@@ -6950,7 +6950,7 @@
         <v>7</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>14</v>
@@ -6958,10 +6958,10 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>14</v>
@@ -6969,10 +6969,10 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>14</v>
@@ -6980,10 +6980,10 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>14</v>
@@ -6991,10 +6991,10 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>14</v>
@@ -7002,10 +7002,10 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>14</v>
@@ -7013,10 +7013,10 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>14</v>
@@ -7024,10 +7024,10 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>14</v>
@@ -7035,10 +7035,10 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>14</v>
@@ -7046,10 +7046,10 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>14</v>
@@ -7057,10 +7057,10 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>14</v>
@@ -7068,10 +7068,10 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>14</v>
@@ -7079,10 +7079,10 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>14</v>
@@ -7090,10 +7090,10 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>14</v>
@@ -7101,10 +7101,10 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>14</v>
@@ -7112,10 +7112,10 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
+        <v>579</v>
+      </c>
+      <c r="B236" s="1" t="s">
         <v>580</v>
-      </c>
-      <c r="B236" s="1" t="s">
-        <v>581</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>14</v>
@@ -7123,10 +7123,10 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>330</v>
@@ -7134,10 +7134,10 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>330</v>
@@ -7145,10 +7145,10 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>330</v>
@@ -7156,10 +7156,10 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C240" s="1" t="s">
         <v>330</v>
@@ -7167,10 +7167,10 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>330</v>
@@ -7178,10 +7178,10 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>330</v>
@@ -7189,10 +7189,10 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>330</v>
@@ -7200,10 +7200,10 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>330</v>
@@ -7211,10 +7211,10 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>330</v>
@@ -7222,10 +7222,10 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>330</v>
@@ -7233,10 +7233,10 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>330</v>
@@ -7244,10 +7244,10 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>330</v>
@@ -7255,10 +7255,10 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>330</v>
@@ -7266,10 +7266,10 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>330</v>
@@ -7280,7 +7280,7 @@
         <v>7</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>330</v>
@@ -7288,10 +7288,10 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>330</v>
@@ -7299,10 +7299,10 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
+        <v>579</v>
+      </c>
+      <c r="B253" s="1" t="s">
         <v>580</v>
-      </c>
-      <c r="B253" s="1" t="s">
-        <v>581</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>330</v>
@@ -7310,101 +7310,101 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed NA to NA1 in lookup beacuse of excel fomrating of NA = NaN
</commit_message>
<xml_diff>
--- a/assets/Inhibtion_Mutations_of_Intrest_2324.xlsx
+++ b/assets/Inhibtion_Mutations_of_Intrest_2324.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Virologi\NGS\1-NGS-Analyser\1-Rutine\2-Resultater\Influensa\Sesongfiler\2324\Mutation_lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866AD703-9862-48E0-9F71-B3C04999FCE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71893E8D-8A23-46BD-BEB9-FEC781FEEC81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{0D809499-6AB2-485B-B1B9-717479A0DA7D}"/>
   </bookViews>
@@ -1679,9 +1679,6 @@
     <t>NI (1/3)</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>T106I;P165L</t>
   </si>
   <si>
@@ -1791,6 +1788,9 @@
   </si>
   <si>
     <t>VICVIC</t>
+  </si>
+  <si>
+    <t>NA1</t>
   </si>
 </sst>
 </file>
@@ -1833,11 +1833,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2155,15 +2159,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5CB93AC-71EE-42C9-B83A-09F5105723E2}">
   <dimension ref="A1:I262"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="E197" sqref="E197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14" style="3" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" customWidth="1"/>
@@ -2175,10 +2179,10 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -2197,17 +2201,17 @@
         <v>217</v>
       </c>
       <c r="I1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -2227,10 +2231,10 @@
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -2250,10 +2254,10 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -2273,10 +2277,10 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -2296,10 +2300,10 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -2319,10 +2323,10 @@
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -2342,10 +2346,10 @@
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -2365,10 +2369,10 @@
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -2388,10 +2392,10 @@
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -2411,10 +2415,10 @@
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -2434,10 +2438,10 @@
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -2457,10 +2461,10 @@
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -2480,10 +2484,10 @@
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="B14" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -2503,10 +2507,10 @@
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="B15" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -2526,10 +2530,10 @@
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="B16" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -2549,10 +2553,10 @@
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="B17" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -2572,10 +2576,10 @@
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="B18" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -2595,10 +2599,10 @@
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="B19" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -2618,10 +2622,10 @@
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="B20" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -2641,10 +2645,10 @@
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="B21" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E21" s="1" t="s">
@@ -2664,10 +2668,10 @@
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="B22" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -2687,10 +2691,10 @@
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="B23" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E23" s="1" t="s">
@@ -2710,10 +2714,10 @@
       <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="B24" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -2733,10 +2737,10 @@
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="B25" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E25" s="1" t="s">
@@ -2756,10 +2760,10 @@
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="B26" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E26" s="1" t="s">
@@ -2779,10 +2783,10 @@
       <c r="A27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="B27" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E27" s="1" t="s">
@@ -2802,10 +2806,10 @@
       <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="B28" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="1" t="s">
@@ -2825,10 +2829,10 @@
       <c r="A29" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="B29" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E29" s="1" t="s">
@@ -2848,10 +2852,10 @@
       <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="B30" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -2871,10 +2875,10 @@
       <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="B31" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E31" s="1" t="s">
@@ -2894,10 +2898,10 @@
       <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="B32" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E32" s="1" t="s">
@@ -2917,10 +2921,10 @@
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C33" s="1" t="s">
+      <c r="B33" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E33" s="1" t="s">
@@ -2940,10 +2944,10 @@
       <c r="A34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="B34" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E34" s="1" t="s">
@@ -2963,10 +2967,10 @@
       <c r="A35" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C35" s="1" t="s">
+      <c r="B35" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E35" s="1" t="s">
@@ -2986,10 +2990,10 @@
       <c r="A36" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="B36" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E36" s="1" t="s">
@@ -3009,10 +3013,10 @@
       <c r="A37" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="B37" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E37" s="1" t="s">
@@ -3032,10 +3036,10 @@
       <c r="A38" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="B38" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E38" s="1" t="s">
@@ -3055,10 +3059,10 @@
       <c r="A39" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="B39" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E39" s="1" t="s">
@@ -3078,10 +3082,10 @@
       <c r="A40" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="B40" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E40" s="1" t="s">
@@ -3101,10 +3105,10 @@
       <c r="A41" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C41" s="1" t="s">
+      <c r="B41" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E41" s="1" t="s">
@@ -3124,10 +3128,10 @@
       <c r="A42" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="B42" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E42" s="1" t="s">
@@ -3147,10 +3151,10 @@
       <c r="A43" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C43" s="1" t="s">
+      <c r="B43" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E43" s="1" t="s">
@@ -3170,10 +3174,10 @@
       <c r="A44" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C44" s="1" t="s">
+      <c r="B44" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E44" s="1" t="s">
@@ -3193,10 +3197,10 @@
       <c r="A45" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="B45" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E45" s="1" t="s">
@@ -3216,10 +3220,10 @@
       <c r="A46" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="B46" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E46" s="1" t="s">
@@ -3239,10 +3243,10 @@
       <c r="A47" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C47" s="1" t="s">
+      <c r="B47" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E47" s="1" t="s">
@@ -3262,10 +3266,10 @@
       <c r="A48" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C48" s="1" t="s">
+      <c r="B48" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E48" s="1" t="s">
@@ -3285,10 +3289,10 @@
       <c r="A49" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C49" s="1" t="s">
+      <c r="B49" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E49" s="1" t="s">
@@ -3308,10 +3312,10 @@
       <c r="A50" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C50" s="1" t="s">
+      <c r="B50" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E50" s="1" t="s">
@@ -3331,10 +3335,10 @@
       <c r="A51" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C51" s="1" t="s">
+      <c r="B51" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E51" s="1" t="s">
@@ -3354,10 +3358,10 @@
       <c r="A52" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C52" s="1" t="s">
+      <c r="B52" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E52" s="1" t="s">
@@ -3377,10 +3381,10 @@
       <c r="A53" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C53" s="1" t="s">
+      <c r="B53" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E53" s="1" t="s">
@@ -3400,10 +3404,10 @@
       <c r="A54" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C54" s="1" t="s">
+      <c r="B54" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E54" s="1" t="s">
@@ -3423,10 +3427,10 @@
       <c r="A55" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C55" s="1" t="s">
+      <c r="B55" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E55" s="1" t="s">
@@ -3446,10 +3450,10 @@
       <c r="A56" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C56" s="1" t="s">
+      <c r="B56" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E56" s="1" t="s">
@@ -3469,10 +3473,10 @@
       <c r="A57" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C57" s="1" t="s">
+      <c r="B57" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E57" s="1" t="s">
@@ -3492,10 +3496,10 @@
       <c r="A58" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C58" s="1" t="s">
+      <c r="B58" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E58" s="1" t="s">
@@ -3515,10 +3519,10 @@
       <c r="A59" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C59" s="1" t="s">
+      <c r="B59" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E59" s="1" t="s">
@@ -3538,10 +3542,10 @@
       <c r="A60" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C60" s="1" t="s">
+      <c r="B60" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E60" s="1" t="s">
@@ -3561,10 +3565,10 @@
       <c r="A61" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C61" s="1" t="s">
+      <c r="B61" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E61" s="1" t="s">
@@ -3584,10 +3588,10 @@
       <c r="A62" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C62" s="1" t="s">
+      <c r="B62" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E62" s="1" t="s">
@@ -3607,10 +3611,10 @@
       <c r="A63" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C63" s="1" t="s">
+      <c r="B63" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E63" s="1" t="s">
@@ -3630,10 +3634,10 @@
       <c r="A64" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C64" s="1" t="s">
+      <c r="B64" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E64" s="1" t="s">
@@ -3653,10 +3657,10 @@
       <c r="A65" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C65" s="1" t="s">
+      <c r="B65" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E65" s="1" t="s">
@@ -3676,10 +3680,10 @@
       <c r="A66" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C66" s="1" t="s">
+      <c r="B66" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E66" s="1" t="s">
@@ -3699,10 +3703,10 @@
       <c r="A67" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C67" s="1" t="s">
+      <c r="B67" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E67" s="1" t="s">
@@ -3722,10 +3726,10 @@
       <c r="A68" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C68" s="1" t="s">
+      <c r="B68" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E68" s="1" t="s">
@@ -3745,10 +3749,10 @@
       <c r="A69" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C69" s="1" t="s">
+      <c r="B69" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D69" s="1"/>
@@ -3769,10 +3773,10 @@
       <c r="A70" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C70" s="1" t="s">
+      <c r="B70" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D70" s="1"/>
@@ -3793,10 +3797,10 @@
       <c r="A71" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C71" s="1" t="s">
+      <c r="B71" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D71" s="1"/>
@@ -3817,10 +3821,10 @@
       <c r="A72" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C72" s="1" t="s">
+      <c r="B72" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D72" s="1"/>
@@ -3841,10 +3845,10 @@
       <c r="A73" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C73" s="1" t="s">
+      <c r="B73" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D73" s="1"/>
@@ -3865,10 +3869,10 @@
       <c r="A74" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C74" s="1" t="s">
+      <c r="B74" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D74" s="1"/>
@@ -3889,10 +3893,10 @@
       <c r="A75" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C75" s="1" t="s">
+      <c r="B75" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D75" s="1"/>
@@ -3913,10 +3917,10 @@
       <c r="A76" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C76" s="1" t="s">
+      <c r="B76" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D76" s="1"/>
@@ -3937,10 +3941,10 @@
       <c r="A77" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C77" s="1" t="s">
+      <c r="B77" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C77" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D77" s="1"/>
@@ -3961,10 +3965,10 @@
       <c r="A78" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C78" s="1" t="s">
+      <c r="B78" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D78" s="1"/>
@@ -3985,10 +3989,10 @@
       <c r="A79" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C79" s="1" t="s">
+      <c r="B79" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D79" s="1"/>
@@ -4009,10 +4013,10 @@
       <c r="A80" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C80" s="1" t="s">
+      <c r="B80" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D80" s="1"/>
@@ -4033,10 +4037,10 @@
       <c r="A81" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C81" s="1" t="s">
+      <c r="B81" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D81" s="1"/>
@@ -4057,10 +4061,10 @@
       <c r="A82" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C82" s="1" t="s">
+      <c r="B82" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D82" s="1"/>
@@ -4081,10 +4085,10 @@
       <c r="A83" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C83" s="1" t="s">
+      <c r="B83" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D83" s="1"/>
@@ -4105,10 +4109,10 @@
       <c r="A84" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C84" s="1" t="s">
+      <c r="B84" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D84" s="1"/>
@@ -4129,10 +4133,10 @@
       <c r="A85" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B85" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C85" s="1" t="s">
+      <c r="B85" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D85" s="1"/>
@@ -4153,10 +4157,10 @@
       <c r="A86" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C86" s="1" t="s">
+      <c r="B86" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C86" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D86" s="1"/>
@@ -4177,10 +4181,10 @@
       <c r="A87" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C87" s="1" t="s">
+      <c r="B87" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D87" s="1"/>
@@ -4201,10 +4205,10 @@
       <c r="A88" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C88" s="1" t="s">
+      <c r="B88" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C88" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D88" s="1"/>
@@ -4225,10 +4229,10 @@
       <c r="A89" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C89" s="1" t="s">
+      <c r="B89" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C89" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D89" s="1"/>
@@ -4249,10 +4253,10 @@
       <c r="A90" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B90" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C90" s="1" t="s">
+      <c r="B90" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C90" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D90" s="1"/>
@@ -4273,10 +4277,10 @@
       <c r="A91" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C91" s="1" t="s">
+      <c r="B91" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D91" s="1"/>
@@ -4297,10 +4301,10 @@
       <c r="A92" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B92" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C92" s="1" t="s">
+      <c r="B92" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E92" s="1" t="s">
@@ -4320,10 +4324,10 @@
       <c r="A93" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C93" s="1" t="s">
+      <c r="B93" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C93" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E93" s="1" t="s">
@@ -4343,10 +4347,10 @@
       <c r="A94" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B94" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C94" s="1" t="s">
+      <c r="B94" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E94" s="1" t="s">
@@ -4366,10 +4370,10 @@
       <c r="A95" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B95" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C95" s="1" t="s">
+      <c r="B95" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E95" s="1" t="s">
@@ -4389,10 +4393,10 @@
       <c r="A96" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="B96" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C96" s="1" t="s">
+      <c r="B96" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E96" s="1" t="s">
@@ -4412,10 +4416,10 @@
       <c r="A97" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B97" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C97" s="1" t="s">
+      <c r="B97" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C97" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E97" s="1" t="s">
@@ -4435,10 +4439,10 @@
       <c r="A98" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C98" s="1" t="s">
+      <c r="B98" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E98" s="1" t="s">
@@ -4458,10 +4462,10 @@
       <c r="A99" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="B99" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C99" s="1" t="s">
+      <c r="B99" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C99" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E99" s="1" t="s">
@@ -4481,10 +4485,10 @@
       <c r="A100" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C100" s="1" t="s">
+      <c r="B100" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C100" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E100" s="1" t="s">
@@ -4504,10 +4508,10 @@
       <c r="A101" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C101" s="1" t="s">
+      <c r="B101" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C101" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E101" s="1" t="s">
@@ -4527,10 +4531,10 @@
       <c r="A102" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B102" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C102" s="1" t="s">
+      <c r="B102" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C102" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E102" s="1" t="s">
@@ -4550,10 +4554,10 @@
       <c r="A103" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="B103" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C103" s="1" t="s">
+      <c r="B103" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C103" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E103" s="1" t="s">
@@ -4573,10 +4577,10 @@
       <c r="A104" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="B104" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C104" s="1" t="s">
+      <c r="B104" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C104" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E104" s="1" t="s">
@@ -4596,10 +4600,10 @@
       <c r="A105" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B105" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C105" s="1" t="s">
+      <c r="B105" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E105" s="1" t="s">
@@ -4619,10 +4623,10 @@
       <c r="A106" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B106" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C106" s="1" t="s">
+      <c r="B106" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C106" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E106" s="1" t="s">
@@ -4642,10 +4646,10 @@
       <c r="A107" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B107" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C107" s="1" t="s">
+      <c r="B107" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C107" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E107" s="1" t="s">
@@ -4665,10 +4669,10 @@
       <c r="A108" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B108" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C108" s="1" t="s">
+      <c r="B108" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C108" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E108" s="1" t="s">
@@ -4688,10 +4692,10 @@
       <c r="A109" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="B109" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C109" s="1" t="s">
+      <c r="B109" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C109" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E109" s="1" t="s">
@@ -4711,10 +4715,10 @@
       <c r="A110" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B110" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C110" s="1" t="s">
+      <c r="B110" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C110" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E110" s="1" t="s">
@@ -4734,10 +4738,10 @@
       <c r="A111" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B111" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C111" s="1" t="s">
+      <c r="B111" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C111" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E111" s="1" t="s">
@@ -4757,10 +4761,10 @@
       <c r="A112" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B112" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C112" s="1" t="s">
+      <c r="B112" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C112" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E112" s="1" t="s">
@@ -4780,10 +4784,10 @@
       <c r="A113" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="B113" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C113" s="1" t="s">
+      <c r="B113" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C113" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E113" s="1" t="s">
@@ -4803,10 +4807,10 @@
       <c r="A114" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="B114" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C114" s="1" t="s">
+      <c r="B114" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C114" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E114" s="1" t="s">
@@ -4826,10 +4830,10 @@
       <c r="A115" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B115" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C115" s="1" t="s">
+      <c r="B115" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C115" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E115" s="1" t="s">
@@ -4849,10 +4853,10 @@
       <c r="A116" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="B116" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C116" s="1" t="s">
+      <c r="B116" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C116" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E116" s="1" t="s">
@@ -4872,10 +4876,10 @@
       <c r="A117" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="B117" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C117" s="1" t="s">
+      <c r="B117" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C117" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E117" s="1" t="s">
@@ -4895,10 +4899,10 @@
       <c r="A118" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="B118" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C118" s="1" t="s">
+      <c r="B118" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C118" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E118" s="1" t="s">
@@ -4918,10 +4922,10 @@
       <c r="A119" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B119" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C119" s="1" t="s">
+      <c r="B119" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C119" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E119" s="1" t="s">
@@ -4941,10 +4945,10 @@
       <c r="A120" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="B120" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C120" s="1" t="s">
+      <c r="B120" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C120" s="2" t="s">
         <v>327</v>
       </c>
       <c r="E120" s="1" t="s">
@@ -4964,10 +4968,10 @@
       <c r="A121" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="B121" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C121" s="1" t="s">
+      <c r="B121" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C121" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E121" s="1" t="s">
@@ -4987,10 +4991,10 @@
       <c r="A122" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="B122" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C122" s="1" t="s">
+      <c r="B122" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C122" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E122" s="1" t="s">
@@ -5010,10 +5014,10 @@
       <c r="A123" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="B123" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C123" s="1" t="s">
+      <c r="B123" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C123" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E123" s="1" t="s">
@@ -5033,10 +5037,10 @@
       <c r="A124" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="B124" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C124" s="1" t="s">
+      <c r="B124" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C124" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E124" s="1" t="s">
@@ -5056,10 +5060,10 @@
       <c r="A125" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="B125" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C125" s="1" t="s">
+      <c r="B125" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C125" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E125" s="1" t="s">
@@ -5079,10 +5083,10 @@
       <c r="A126" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="B126" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C126" s="1" t="s">
+      <c r="B126" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C126" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E126" s="1" t="s">
@@ -5102,10 +5106,10 @@
       <c r="A127" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B127" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C127" s="1" t="s">
+      <c r="B127" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C127" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E127" s="1" t="s">
@@ -5125,10 +5129,10 @@
       <c r="A128" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="B128" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C128" s="1" t="s">
+      <c r="B128" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C128" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E128" s="1" t="s">
@@ -5148,10 +5152,10 @@
       <c r="A129" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="B129" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C129" s="1" t="s">
+      <c r="B129" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C129" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E129" s="1" t="s">
@@ -5171,10 +5175,10 @@
       <c r="A130" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="B130" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C130" s="1" t="s">
+      <c r="B130" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C130" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E130" s="1" t="s">
@@ -5194,10 +5198,10 @@
       <c r="A131" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="B131" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C131" s="1" t="s">
+      <c r="B131" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C131" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E131" s="1" t="s">
@@ -5217,10 +5221,10 @@
       <c r="A132" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="B132" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C132" s="1" t="s">
+      <c r="B132" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C132" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E132" s="1" t="s">
@@ -5240,10 +5244,10 @@
       <c r="A133" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="B133" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C133" s="1" t="s">
+      <c r="B133" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C133" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E133" s="1" t="s">
@@ -5263,10 +5267,10 @@
       <c r="A134" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="B134" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C134" s="1" t="s">
+      <c r="B134" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C134" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E134" s="1" t="s">
@@ -5286,10 +5290,10 @@
       <c r="A135" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="B135" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C135" s="1" t="s">
+      <c r="B135" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C135" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E135" s="1" t="s">
@@ -5309,10 +5313,10 @@
       <c r="A136" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="B136" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C136" s="1" t="s">
+      <c r="B136" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C136" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E136" s="1" t="s">
@@ -5332,11 +5336,11 @@
       <c r="A137" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="B137" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>584</v>
+      <c r="B137" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>438</v>
@@ -5355,11 +5359,11 @@
       <c r="A138" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="B138" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>584</v>
+      <c r="B138" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>442</v>
@@ -5378,11 +5382,11 @@
       <c r="A139" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="B139" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>584</v>
+      <c r="B139" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>446</v>
@@ -5401,11 +5405,11 @@
       <c r="A140" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="B140" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>584</v>
+      <c r="B140" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>450</v>
@@ -5424,11 +5428,11 @@
       <c r="A141" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="B141" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C141" s="1" t="s">
-        <v>584</v>
+      <c r="B141" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>454</v>
@@ -5447,11 +5451,11 @@
       <c r="A142" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="B142" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>584</v>
+      <c r="B142" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>458</v>
@@ -5470,11 +5474,11 @@
       <c r="A143" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="B143" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C143" s="1" t="s">
-        <v>584</v>
+      <c r="B143" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>461</v>
@@ -5493,11 +5497,11 @@
       <c r="A144" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="B144" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>584</v>
+      <c r="B144" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>212</v>
@@ -5516,11 +5520,11 @@
       <c r="A145" t="s">
         <v>397</v>
       </c>
-      <c r="B145" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C145" s="1" t="s">
-        <v>584</v>
+      <c r="B145" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E145" t="s">
         <v>326</v>
@@ -5539,11 +5543,11 @@
       <c r="A146" t="s">
         <v>398</v>
       </c>
-      <c r="B146" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>584</v>
+      <c r="B146" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E146" t="s">
         <v>102</v>
@@ -5562,11 +5566,11 @@
       <c r="A147" t="s">
         <v>399</v>
       </c>
-      <c r="B147" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>584</v>
+      <c r="B147" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E147" t="s">
         <v>108</v>
@@ -5585,11 +5589,11 @@
       <c r="A148" t="s">
         <v>400</v>
       </c>
-      <c r="B148" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>584</v>
+      <c r="B148" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E148" t="s">
         <v>74</v>
@@ -5608,11 +5612,11 @@
       <c r="A149" t="s">
         <v>401</v>
       </c>
-      <c r="B149" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C149" s="1" t="s">
-        <v>584</v>
+      <c r="B149" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E149" t="s">
         <v>472</v>
@@ -5631,11 +5635,11 @@
       <c r="A150" t="s">
         <v>402</v>
       </c>
-      <c r="B150" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C150" s="1" t="s">
-        <v>584</v>
+      <c r="B150" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E150" t="s">
         <v>476</v>
@@ -5654,11 +5658,11 @@
       <c r="A151" t="s">
         <v>403</v>
       </c>
-      <c r="B151" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C151" s="1" t="s">
-        <v>584</v>
+      <c r="B151" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E151" t="s">
         <v>105</v>
@@ -5677,11 +5681,11 @@
       <c r="A152" t="s">
         <v>404</v>
       </c>
-      <c r="B152" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>584</v>
+      <c r="B152" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E152" t="s">
         <v>74</v>
@@ -5700,11 +5704,11 @@
       <c r="A153" t="s">
         <v>405</v>
       </c>
-      <c r="B153" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>584</v>
+      <c r="B153" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E153" t="s">
         <v>438</v>
@@ -5723,11 +5727,11 @@
       <c r="A154" t="s">
         <v>406</v>
       </c>
-      <c r="B154" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C154" s="1" t="s">
-        <v>584</v>
+      <c r="B154" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E154" t="s">
         <v>105</v>
@@ -5746,11 +5750,11 @@
       <c r="A155" t="s">
         <v>407</v>
       </c>
-      <c r="B155" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C155" s="1" t="s">
-        <v>584</v>
+      <c r="B155" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E155" t="s">
         <v>483</v>
@@ -5769,11 +5773,11 @@
       <c r="A156" t="s">
         <v>408</v>
       </c>
-      <c r="B156" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>584</v>
+      <c r="B156" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E156" t="s">
         <v>487</v>
@@ -5792,11 +5796,11 @@
       <c r="A157" t="s">
         <v>409</v>
       </c>
-      <c r="B157" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>584</v>
+      <c r="B157" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E157" t="s">
         <v>490</v>
@@ -5815,11 +5819,11 @@
       <c r="A158" t="s">
         <v>410</v>
       </c>
-      <c r="B158" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>584</v>
+      <c r="B158" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E158" t="s">
         <v>74</v>
@@ -5838,11 +5842,11 @@
       <c r="A159" t="s">
         <v>411</v>
       </c>
-      <c r="B159" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>584</v>
+      <c r="B159" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E159" t="s">
         <v>322</v>
@@ -5861,11 +5865,11 @@
       <c r="A160" t="s">
         <v>412</v>
       </c>
-      <c r="B160" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>584</v>
+      <c r="B160" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E160" t="s">
         <v>469</v>
@@ -5884,11 +5888,11 @@
       <c r="A161" t="s">
         <v>413</v>
       </c>
-      <c r="B161" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>584</v>
+      <c r="B161" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E161" t="s">
         <v>105</v>
@@ -5907,11 +5911,11 @@
       <c r="A162" t="s">
         <v>414</v>
       </c>
-      <c r="B162" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>584</v>
+      <c r="B162" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E162" t="s">
         <v>494</v>
@@ -5930,11 +5934,11 @@
       <c r="A163" t="s">
         <v>415</v>
       </c>
-      <c r="B163" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>584</v>
+      <c r="B163" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E163" t="s">
         <v>102</v>
@@ -5953,11 +5957,11 @@
       <c r="A164" t="s">
         <v>416</v>
       </c>
-      <c r="B164" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>584</v>
+      <c r="B164" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E164" t="s">
         <v>446</v>
@@ -5976,11 +5980,11 @@
       <c r="A165" t="s">
         <v>417</v>
       </c>
-      <c r="B165" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>584</v>
+      <c r="B165" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E165" t="s">
         <v>499</v>
@@ -5999,11 +6003,11 @@
       <c r="A166" t="s">
         <v>418</v>
       </c>
-      <c r="B166" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C166" s="1" t="s">
-        <v>584</v>
+      <c r="B166" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E166" t="s">
         <v>501</v>
@@ -6022,11 +6026,11 @@
       <c r="A167" t="s">
         <v>419</v>
       </c>
-      <c r="B167" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C167" s="1" t="s">
-        <v>584</v>
+      <c r="B167" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E167" t="s">
         <v>505</v>
@@ -6045,11 +6049,11 @@
       <c r="A168" t="s">
         <v>420</v>
       </c>
-      <c r="B168" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>584</v>
+      <c r="B168" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E168" t="s">
         <v>508</v>
@@ -6068,11 +6072,11 @@
       <c r="A169" t="s">
         <v>421</v>
       </c>
-      <c r="B169" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C169" s="1" t="s">
-        <v>584</v>
+      <c r="B169" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E169" t="s">
         <v>511</v>
@@ -6091,11 +6095,11 @@
       <c r="A170" t="s">
         <v>422</v>
       </c>
-      <c r="B170" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C170" s="1" t="s">
-        <v>584</v>
+      <c r="B170" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E170" t="s">
         <v>105</v>
@@ -6114,11 +6118,11 @@
       <c r="A171" t="s">
         <v>423</v>
       </c>
-      <c r="B171" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>584</v>
+      <c r="B171" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E171" t="s">
         <v>516</v>
@@ -6137,11 +6141,11 @@
       <c r="A172" t="s">
         <v>424</v>
       </c>
-      <c r="B172" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C172" s="1" t="s">
-        <v>584</v>
+      <c r="B172" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E172" t="s">
         <v>105</v>
@@ -6160,11 +6164,11 @@
       <c r="A173" t="s">
         <v>425</v>
       </c>
-      <c r="B173" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C173" s="1" t="s">
-        <v>584</v>
+      <c r="B173" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E173" t="s">
         <v>108</v>
@@ -6183,11 +6187,11 @@
       <c r="A174" t="s">
         <v>426</v>
       </c>
-      <c r="B174" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C174" s="1" t="s">
-        <v>584</v>
+      <c r="B174" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E174" t="s">
         <v>521</v>
@@ -6206,11 +6210,11 @@
       <c r="A175" t="s">
         <v>11</v>
       </c>
-      <c r="B175" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C175" s="1" t="s">
-        <v>584</v>
+      <c r="B175" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E175" t="s">
         <v>458</v>
@@ -6229,11 +6233,11 @@
       <c r="A176" t="s">
         <v>12</v>
       </c>
-      <c r="B176" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C176" s="1" t="s">
-        <v>584</v>
+      <c r="B176" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E176" t="s">
         <v>524</v>
@@ -6252,11 +6256,11 @@
       <c r="A177" t="s">
         <v>427</v>
       </c>
-      <c r="B177" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C177" s="1" t="s">
-        <v>584</v>
+      <c r="B177" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E177" t="s">
         <v>105</v>
@@ -6275,11 +6279,11 @@
       <c r="A178" t="s">
         <v>428</v>
       </c>
-      <c r="B178" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>584</v>
+      <c r="B178" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E178" t="s">
         <v>105</v>
@@ -6298,11 +6302,11 @@
       <c r="A179" t="s">
         <v>429</v>
       </c>
-      <c r="B179" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C179" s="1" t="s">
-        <v>584</v>
+      <c r="B179" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E179" t="s">
         <v>528</v>
@@ -6321,11 +6325,11 @@
       <c r="A180" t="s">
         <v>430</v>
       </c>
-      <c r="B180" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C180" s="1" t="s">
-        <v>584</v>
+      <c r="B180" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E180" t="s">
         <v>322</v>
@@ -6344,11 +6348,11 @@
       <c r="A181" t="s">
         <v>431</v>
       </c>
-      <c r="B181" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C181" s="1" t="s">
-        <v>584</v>
+      <c r="B181" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E181" t="s">
         <v>102</v>
@@ -6367,11 +6371,11 @@
       <c r="A182" t="s">
         <v>432</v>
       </c>
-      <c r="B182" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C182" s="1" t="s">
-        <v>584</v>
+      <c r="B182" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E182" t="s">
         <v>108</v>
@@ -6390,11 +6394,11 @@
       <c r="A183" t="s">
         <v>433</v>
       </c>
-      <c r="B183" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C183" s="1" t="s">
-        <v>584</v>
+      <c r="B183" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E183" t="s">
         <v>74</v>
@@ -6413,11 +6417,11 @@
       <c r="A184" t="s">
         <v>434</v>
       </c>
-      <c r="B184" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C184" s="1" t="s">
-        <v>584</v>
+      <c r="B184" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E184" t="s">
         <v>74</v>
@@ -6436,11 +6440,11 @@
       <c r="A185" t="s">
         <v>435</v>
       </c>
-      <c r="B185" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C185" s="1" t="s">
-        <v>584</v>
+      <c r="B185" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E185" t="s">
         <v>533</v>
@@ -6459,11 +6463,11 @@
       <c r="A186" t="s">
         <v>436</v>
       </c>
-      <c r="B186" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C186" s="1" t="s">
-        <v>584</v>
+      <c r="B186" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E186" t="s">
         <v>74</v>
@@ -6482,11 +6486,11 @@
       <c r="A187" t="s">
         <v>437</v>
       </c>
-      <c r="B187" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C187" s="1" t="s">
-        <v>584</v>
+      <c r="B187" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E187" t="s">
         <v>74</v>
@@ -6503,13 +6507,13 @@
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>548</v>
-      </c>
-      <c r="B188" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="C188" s="1" t="s">
-        <v>584</v>
+      <c r="B188" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E188" t="s">
         <v>108</v>
@@ -6526,13 +6530,13 @@
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>549</v>
-      </c>
-      <c r="B189" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C189" s="1" t="s">
-        <v>584</v>
+        <v>548</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E189" t="s">
         <v>104</v>
@@ -6549,13 +6553,13 @@
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>550</v>
-      </c>
-      <c r="B190" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C190" s="1" t="s">
-        <v>584</v>
+        <v>549</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E190" t="s">
         <v>322</v>
@@ -6572,13 +6576,13 @@
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>551</v>
-      </c>
-      <c r="B191" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C191" s="1" t="s">
-        <v>584</v>
+        <v>550</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E191" t="s">
         <v>539</v>
@@ -6595,13 +6599,13 @@
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>552</v>
-      </c>
-      <c r="B192" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C192" s="1" t="s">
-        <v>584</v>
+        <v>551</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E192" t="s">
         <v>102</v>
@@ -6618,13 +6622,13 @@
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>553</v>
-      </c>
-      <c r="B193" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C193" s="1" t="s">
-        <v>584</v>
+        <v>552</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="E193" t="s">
         <v>543</v>
@@ -6641,298 +6645,298 @@
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>554</v>
-      </c>
-      <c r="B194" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="C194" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C194" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>555</v>
-      </c>
-      <c r="B195" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="C195" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C195" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>556</v>
-      </c>
-      <c r="B196" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="C196" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C196" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>557</v>
-      </c>
-      <c r="B197" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="C197" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C197" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>558</v>
-      </c>
-      <c r="B198" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="C198" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C198" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>559</v>
-      </c>
-      <c r="B199" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="C199" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C199" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>554</v>
-      </c>
-      <c r="B200" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="C200" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C200" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>555</v>
-      </c>
-      <c r="B201" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="C201" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C201" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>556</v>
-      </c>
-      <c r="B202" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="C202" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C202" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>557</v>
-      </c>
-      <c r="B203" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="C203" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C203" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>558</v>
-      </c>
-      <c r="B204" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="C204" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C204" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>559</v>
-      </c>
-      <c r="B205" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="C205" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C205" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>554</v>
-      </c>
-      <c r="B206" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="C206" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C206" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>555</v>
-      </c>
-      <c r="B207" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="C207" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C207" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>556</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="C208" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C208" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>557</v>
-      </c>
-      <c r="B209" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="C209" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C209" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>558</v>
-      </c>
-      <c r="B210" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="C210" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C210" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>559</v>
-      </c>
-      <c r="B211" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="C211" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C211" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>561</v>
-      </c>
-      <c r="B212" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C212" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C212" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>562</v>
-      </c>
-      <c r="B213" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C213" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C213" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>563</v>
-      </c>
-      <c r="B214" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C214" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C214" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>564</v>
-      </c>
-      <c r="B215" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C215" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C215" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>565</v>
-      </c>
-      <c r="B216" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C216" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C216" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>566</v>
-      </c>
-      <c r="B217" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C217" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C217" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>567</v>
-      </c>
-      <c r="B218" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C218" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C218" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>568</v>
-      </c>
-      <c r="B219" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C219" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C219" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>569</v>
-      </c>
-      <c r="B220" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C220" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C220" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6940,329 +6944,329 @@
       <c r="A221" t="s">
         <v>7</v>
       </c>
-      <c r="B221" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C221" s="1" t="s">
+      <c r="B221" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C221" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>570</v>
-      </c>
-      <c r="B222" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C222" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C222" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>571</v>
-      </c>
-      <c r="B223" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C223" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C223" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>561</v>
-      </c>
-      <c r="B224" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C224" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C224" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>572</v>
-      </c>
-      <c r="B225" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C225" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C225" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>573</v>
-      </c>
-      <c r="B226" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C226" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C226" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>574</v>
-      </c>
-      <c r="B227" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C227" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C227" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>563</v>
-      </c>
-      <c r="B228" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C228" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C228" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>564</v>
-      </c>
-      <c r="B229" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C229" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C229" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>565</v>
-      </c>
-      <c r="B230" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C230" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C230" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>567</v>
-      </c>
-      <c r="B231" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C231" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C231" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>568</v>
-      </c>
-      <c r="B232" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C232" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C232" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>569</v>
-      </c>
-      <c r="B233" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C233" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C233" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>570</v>
-      </c>
-      <c r="B234" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C234" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C234" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>575</v>
-      </c>
-      <c r="B235" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C235" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C235" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
+        <v>575</v>
+      </c>
+      <c r="B236" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="B236" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C236" s="1" t="s">
+      <c r="C236" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>578</v>
-      </c>
-      <c r="B237" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="C237" s="1" t="s">
+      <c r="B237" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C237" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>571</v>
-      </c>
-      <c r="B238" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C238" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C238" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>561</v>
-      </c>
-      <c r="B239" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C239" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C239" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>572</v>
-      </c>
-      <c r="B240" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C240" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C240" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>573</v>
-      </c>
-      <c r="B241" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C241" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C241" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>562</v>
-      </c>
-      <c r="B242" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C242" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C242" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>574</v>
-      </c>
-      <c r="B243" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C243" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C243" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>563</v>
-      </c>
-      <c r="B244" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C244" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C244" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>564</v>
-      </c>
-      <c r="B245" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C245" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C245" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>565</v>
-      </c>
-      <c r="B246" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C246" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C246" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>566</v>
-      </c>
-      <c r="B247" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C247" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="B247" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C247" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>567</v>
-      </c>
-      <c r="B248" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C248" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="B248" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C248" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>568</v>
-      </c>
-      <c r="B249" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C249" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="B249" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C249" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>569</v>
-      </c>
-      <c r="B250" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C250" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C250" s="2" t="s">
         <v>327</v>
       </c>
     </row>
@@ -7270,132 +7274,132 @@
       <c r="A251" t="s">
         <v>7</v>
       </c>
-      <c r="B251" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C251" s="1" t="s">
+      <c r="B251" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C251" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>570</v>
-      </c>
-      <c r="B252" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C252" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C252" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
+        <v>575</v>
+      </c>
+      <c r="B253" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="B253" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C253" s="1" t="s">
+      <c r="C253" s="2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>561</v>
-      </c>
-      <c r="B254" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C254" s="1" t="s">
-        <v>584</v>
+        <v>560</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>579</v>
-      </c>
-      <c r="B255" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C255" s="1" t="s">
-        <v>584</v>
+        <v>578</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C255" s="2" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>581</v>
-      </c>
-      <c r="B256" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C256" s="1" t="s">
-        <v>584</v>
+        <v>580</v>
+      </c>
+      <c r="B256" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>563</v>
-      </c>
-      <c r="B257" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C257" s="1" t="s">
-        <v>584</v>
+        <v>562</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>565</v>
-      </c>
-      <c r="B258" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C258" s="1" t="s">
-        <v>584</v>
+        <v>564</v>
+      </c>
+      <c r="B258" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>568</v>
-      </c>
-      <c r="B259" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C259" s="1" t="s">
-        <v>584</v>
+        <v>567</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>569</v>
-      </c>
-      <c r="B260" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C260" s="1" t="s">
-        <v>584</v>
+        <v>568</v>
+      </c>
+      <c r="B260" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>582</v>
-      </c>
-      <c r="B261" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C261" s="1" t="s">
-        <v>584</v>
+        <v>581</v>
+      </c>
+      <c r="B261" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>580</v>
-      </c>
-      <c r="B262" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C262" s="1" t="s">
-        <v>584</v>
+        <v>579</v>
+      </c>
+      <c r="B262" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>